<commit_message>
Init repo for sim on 47
</commit_message>
<xml_diff>
--- a/fitters/cluster_dynamics.xlsx
+++ b/fitters/cluster_dynamics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Github\vegetation-dynamics\fitters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BE3400-7675-487C-8CB5-1A3B4DFBB373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BBC292-4688-42EE-A115-7097C7392122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,14 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +485,7 @@
   <dimension ref="B2:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,30 +494,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -568,13 +573,13 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>208.13742869917201</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>160.816435853033</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>165.30673929495401</v>
       </c>
       <c r="G4" t="s">
@@ -618,13 +623,13 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>242.033611139279</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>187.342705699552</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>192.478019023668</v>
       </c>
       <c r="G5" t="s">
@@ -668,13 +673,13 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>336.15105358667802</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>261.26288008767602</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>268.06289318057298</v>
       </c>
       <c r="G6" t="s">
@@ -718,13 +723,13 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>459.92761213935501</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>358.90552709623302</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>367.70074833581299</v>
       </c>
       <c r="G7" t="s">
@@ -768,13 +773,13 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>668.68489258357499</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>524.31193950762395</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>536.167605780705</v>
       </c>
       <c r="G8" t="s">
@@ -818,13 +823,13 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>1172.06041249348</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>1141.9656539969101</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>943.790513379603</v>
       </c>
       <c r="G9" t="s">
@@ -865,16 +870,16 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>1586.4144793294599</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>1280.31509015097</v>
       </c>
       <c r="G10" t="s">
@@ -889,16 +894,16 @@
       <c r="J10">
         <v>19671.835770000002</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="1">
         <v>4653.0622320000002</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="1">
         <v>4547.6322550000004</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="1">
         <v>3784.8393310000001</v>
       </c>
       <c r="Q10" t="s">
@@ -915,16 +920,16 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>26535.633196560499</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>25790.2027165371</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>21856.6727759284</v>
       </c>
       <c r="G11" t="s">
@@ -953,42 +958,42 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>51199.110539033303</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>49435.268787219298</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>42368.117716030298</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="1">
         <v>25235.513889999998</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="1">
         <v>24538.33152</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="1">
         <v>20778.350190000001</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="1">
         <v>53734.979700000004</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="1">
         <v>51857.498200000002</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="1">
         <v>44481.695110000001</v>
       </c>
     </row>

</xml_diff>